<commit_message>
updated news and achievements excel sheet
</commit_message>
<xml_diff>
--- a/assets/news/qualiperf_news.xlsx
+++ b/assets/news/qualiperf_news.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helen\Desktop\Uni\Github\Qualiperf.github.io\qualiperf.github.io\assets\news\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A5A19D-44ED-4DE8-A60B-D2D34CA7B997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3951A910-F16C-4A60-9ACB-0081A01D54A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="744">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2727,6 +2727,72 @@
   </si>
   <si>
     <t xml:space="preserve">10.3389/fbioe.2023.1179980 </t>
+  </si>
+  <si>
+    <t>Automated Detection of Portal Fields and Central Veins in Whole-Slide Images of Liver Tissue</t>
+  </si>
+  <si>
+    <t>Budelmann D, Laue H, Weis N, Dahmen U, D’Alessandro LA, Biermayer I, Klingmüller U, Ghallab A, Hassan R, Begher-Tibbe B, Hengstler JG, Schwen LO</t>
+  </si>
+  <si>
+    <t>Many physiological processes and pathological phenomena in the liver tissue are spatially heterogeneous. At a local scale, biomarkers can be quantified along the axis of the blood flow, from portal fields (PFs) to central veins (CVs), i.e., in zonated form. This requires detecting PFs and CVs. However, manually annotating these structures in multiple whole-slide images is a tedious task. We describe and evaluate a fully automated method, based on a convolutional neural network, for simultaneously detecting PFs and CVs in a single stained section. Trained on scans of hematoxylin and eosin-stained liver tissue, the detector performed well with an F1 score of 0.81 compared to annotation by a human expert. It does, however, not generalize well to previously unseen scans of steatotic liver tissue with an F1 score of 0.59. Automated PF and CV detection eliminates the bottleneck of manual annotation for subsequent automated analyses, as illustrated by two proof-of-concept applications: We computed lobulus sizes based on the detected PF and CV positions, where results agreed with published lobulus sizes. Moreover, we demonstrate the feasibility of zonated quantification of biomarkers detected in different stainings based on lobuli and zones obtained from the detected PF and CV positions. A negative control (hematoxylin and eosin) showed the expected homogeneity, a positive control (glutamine synthetase) was quantified to be strictly pericentral, and a plausible zonation for a heterogeneous F4/80 staining was obtained. Automated detection of PFs and CVs is one building block for automatically quantifying physiologically relevant heterogeneity of liver tissue biomarkers. Perspectively, a more robust and automated assessment of zonation from whole-slide images will be valuable for parameterizing spatially resolved models of liver metabolism and to provide diagnostic information.</t>
+  </si>
+  <si>
+    <t>Journal of Pathology Informatics 2022 13:100001, doi: 10.1016/j.jpi.2022.100001</t>
+  </si>
+  <si>
+    <t>2/14/2022</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1qmU_QTNS3-U0odNaQclebHO2u52FOHkS</t>
+  </si>
+  <si>
+    <t>(None received QuaLiPerF funding for this work)</t>
+  </si>
+  <si>
+    <t>Zenodo</t>
+  </si>
+  <si>
+    <t>Data, Code</t>
+  </si>
+  <si>
+    <t>Stea-PK Mod</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Datasets for "Automated Detection of Portal Fields and Central Veins in Whole-Slide Images of Liver Tissue"</t>
+  </si>
+  <si>
+    <t>Datasets and results for the manuscript “Automated Detection of Portal Fields and Central Veins in Whole-Slide Images of Liver Tissue” (Journal of Pathology Informatics 13 (2022) 100001, https://doi.org/10.1016/j.jpi.2022.100001)</t>
+  </si>
+  <si>
+    <t>Zenodo 2022, doi: 10.5281/zenodo.5726769</t>
+  </si>
+  <si>
+    <t>Segmentation of Lipid Droplets in Histological Images</t>
+  </si>
+  <si>
+    <t>Budelmann D, Cao Q, Laue H, Albadry M, Dahmen U, Schwen LO</t>
+  </si>
+  <si>
+    <t>Steatosis is a common liver disease characterized by the accumulation of lipid droplets in cells. Precise and reliable fat droplet identification is essential for automatic steatosis quantification in histological images. We trained a nnU-Net to automatically segment lipid vacuoles in whole-slide images using semi-automatically generated reference annotations. We evaluated the performance of the trained model on two out-of-distribution datasets. The trained model’s average F1 scores (0.801 and 0.804) suggest a high potential of the nnU-Net framework for the automatic segmentation of lipid vacuoles.</t>
+  </si>
+  <si>
+    <t>Medical Imaging with Deep Learning MIDL 2023, https://2023.midl.io/</t>
+  </si>
+  <si>
+    <t>Data, code</t>
+  </si>
+  <si>
+    <t>Dataset for "Segmentation of Lipid Droplets in Histological Images"</t>
+  </si>
+  <si>
+    <t>Datasets for the publication "Segmentation of Lipid Droplets in Histological Images" (submitted)</t>
+  </si>
+  <si>
+    <t>Zenodo 2023, doi: 10.5281/zenodo.7802211</t>
   </si>
 </sst>
 </file>
@@ -2898,7 +2964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3037,6 +3103,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10664,8 +10739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12266,32 +12341,64 @@
       <c r="Z30" s="46"/>
       <c r="AA30" s="46"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
+    <row r="31" spans="1:27" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="54">
+        <v>45265.410578703704</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>722</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>723</v>
+      </c>
+      <c r="F31" s="46" t="s">
+        <v>724</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>725</v>
+      </c>
+      <c r="H31" s="46"/>
+      <c r="I31" s="48" t="s">
+        <v>726</v>
+      </c>
+      <c r="J31" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K31" s="49" t="s">
+        <v>727</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>728</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="N31" s="46" t="s">
+        <v>729</v>
+      </c>
+      <c r="O31" s="46" t="s">
+        <v>730</v>
+      </c>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="46"/>
+      <c r="V31" s="46"/>
+      <c r="W31" s="46"/>
+      <c r="X31" s="46"/>
+      <c r="Y31" s="46"/>
+      <c r="Z31" s="46"/>
+      <c r="AA31" s="46"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
@@ -14857,9 +14964,10 @@
     <hyperlink ref="K29" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
     <hyperlink ref="K30" r:id="rId22" xr:uid="{495057DF-2B1C-4385-ADFB-55D6A8A151DF}"/>
     <hyperlink ref="S30" r:id="rId23" display="https://doi.org/10.3389/fbioe.2023.1179980" xr:uid="{79C24F57-0DBE-48F6-BE5F-139B44D1E7CC}"/>
+    <hyperlink ref="K31" r:id="rId24" xr:uid="{3035AAD5-AD1A-47B4-A065-757BF07E623F}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -18416,9 +18524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18437,7 +18545,7 @@
     <col min="25" max="1024" width="12.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -18497,7 +18605,7 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
     </row>
-    <row r="2" spans="1:24" ht="35.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="35.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>44665.383020370398</v>
       </c>
@@ -18547,33 +18655,64 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="53">
+        <v>45265.423993055556</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>736</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>737</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>738</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
+        <v>739</v>
+      </c>
+      <c r="I3" s="55">
+        <v>45081</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46" t="s">
+        <v>728</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>729</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>740</v>
+      </c>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -18599,7 +18738,7 @@
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -18625,7 +18764,7 @@
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -18651,7 +18790,7 @@
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -18677,7 +18816,7 @@
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -18703,7 +18842,7 @@
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -18729,7 +18868,7 @@
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -18755,7 +18894,7 @@
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -18781,7 +18920,7 @@
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -18807,7 +18946,7 @@
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -18833,7 +18972,7 @@
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -18859,7 +18998,7 @@
       <c r="W14" s="9"/>
       <c r="X14" s="9"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -18885,7 +19024,7 @@
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -21162,9 +21301,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ163"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:AA66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -23708,7 +23847,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:24" s="45" customFormat="1" ht="337.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" s="45" customFormat="1" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="42" t="s">
         <v>708</v>
       </c>
@@ -23756,59 +23895,109 @@
       <c r="W64" s="43"/>
       <c r="X64" s="43"/>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="8"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="9"/>
-      <c r="S65" s="9"/>
-      <c r="T65" s="9"/>
-      <c r="U65" s="9"/>
-      <c r="V65" s="9"/>
-      <c r="W65" s="9"/>
-      <c r="X65" s="9"/>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="8"/>
-      <c r="P66" s="8"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="9"/>
-      <c r="S66" s="9"/>
-      <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-      <c r="V66" s="9"/>
-      <c r="W66" s="9"/>
-      <c r="X66" s="9"/>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="54">
+        <v>45265.412118055552</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>732</v>
+      </c>
+      <c r="D65" s="46" t="s">
+        <v>733</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>723</v>
+      </c>
+      <c r="F65" s="46" t="s">
+        <v>734</v>
+      </c>
+      <c r="G65" s="47" t="s">
+        <v>735</v>
+      </c>
+      <c r="H65" s="46"/>
+      <c r="I65" s="55">
+        <v>44420</v>
+      </c>
+      <c r="J65" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K65" s="46"/>
+      <c r="L65" s="47" t="s">
+        <v>728</v>
+      </c>
+      <c r="M65" s="46"/>
+      <c r="N65" s="46"/>
+      <c r="O65" s="46"/>
+      <c r="P65" s="46"/>
+      <c r="Q65" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="R65" s="46"/>
+      <c r="S65" s="46"/>
+      <c r="T65" s="46"/>
+      <c r="U65" s="46"/>
+      <c r="V65" s="46"/>
+      <c r="W65" s="46"/>
+      <c r="X65" s="46"/>
+      <c r="Y65" s="46"/>
+      <c r="Z65" s="46"/>
+      <c r="AA65" s="46"/>
+    </row>
+    <row r="66" spans="1:27" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="53">
+        <v>45265.425995370373</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>732</v>
+      </c>
+      <c r="D66" s="46" t="s">
+        <v>741</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>737</v>
+      </c>
+      <c r="F66" s="46" t="s">
+        <v>742</v>
+      </c>
+      <c r="G66" s="47" t="s">
+        <v>743</v>
+      </c>
+      <c r="H66" s="46"/>
+      <c r="I66" s="55">
+        <v>45050</v>
+      </c>
+      <c r="J66" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K66" s="46"/>
+      <c r="L66" s="47" t="s">
+        <v>728</v>
+      </c>
+      <c r="M66" s="46"/>
+      <c r="N66" s="46"/>
+      <c r="O66" s="46"/>
+      <c r="P66" s="46"/>
+      <c r="Q66" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="R66" s="46"/>
+      <c r="S66" s="46"/>
+      <c r="T66" s="46"/>
+      <c r="U66" s="46"/>
+      <c r="V66" s="46"/>
+      <c r="W66" s="46"/>
+      <c r="X66" s="46"/>
+      <c r="Y66" s="46"/>
+      <c r="Z66" s="46"/>
+      <c r="AA66" s="46"/>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -23834,7 +24023,7 @@
       <c r="W67" s="9"/>
       <c r="X67" s="9"/>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -23860,7 +24049,7 @@
       <c r="W68" s="9"/>
       <c r="X68" s="9"/>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -23886,7 +24075,7 @@
       <c r="W69" s="9"/>
       <c r="X69" s="9"/>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -23912,7 +24101,7 @@
       <c r="W70" s="9"/>
       <c r="X70" s="9"/>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -23938,7 +24127,7 @@
       <c r="W71" s="9"/>
       <c r="X71" s="9"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -23964,7 +24153,7 @@
       <c r="W72" s="9"/>
       <c r="X72" s="9"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -23990,7 +24179,7 @@
       <c r="W73" s="9"/>
       <c r="X73" s="9"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -24016,7 +24205,7 @@
       <c r="W74" s="9"/>
       <c r="X74" s="9"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -24042,7 +24231,7 @@
       <c r="W75" s="9"/>
       <c r="X75" s="9"/>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -24068,7 +24257,7 @@
       <c r="W76" s="9"/>
       <c r="X76" s="9"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -24094,7 +24283,7 @@
       <c r="W77" s="9"/>
       <c r="X77" s="9"/>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -24120,7 +24309,7 @@
       <c r="W78" s="9"/>
       <c r="X78" s="9"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -24146,7 +24335,7 @@
       <c r="W79" s="9"/>
       <c r="X79" s="9"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>

</xml_diff>

<commit_message>
updated news and achievements
</commit_message>
<xml_diff>
--- a/assets/news/qualiperf_news.xlsx
+++ b/assets/news/qualiperf_news.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Github\Qualiperf.github.io\qualiperf.github.io\assets\news\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484F6BE7-F327-46CE-8850-39292C62A776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B88186-E3C0-4A5A-B335-28B56A44D51B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="818">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2990,6 +2990,82 @@
   </si>
   <si>
     <t>10.1002/jmri.28698</t>
+  </si>
+  <si>
+    <t>laura.buetow@uni-jena.de</t>
+  </si>
+  <si>
+    <t>The influence of marginal organs on the drug metabolism in liver transplantation</t>
+  </si>
+  <si>
+    <t>Bütow L.B., Tautenhahn H.-M. T., Schröter D.S., Schlattmann P.S., Settmacher U.S., Dahmen U.D.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background and Aims: 
+Metabolic zonation is a liver phenomenon, described as different distribution of functions among lobules. One liver function is the degradation of drugs, which is realized by cytochrome P450 enzymes. The alteration of CYP expression and activity will be studied in marginal donor livers for a better characterization of these high-risk organs to improve the graft selection process.
+Method: 
+The first step of the study is to investigate the influence of marginal organs on drug metabolism, by comparing the steatosis severity, the donor age, and the CIT to the CYP expression and activity. The measurements will be correlated to the change in reperfusion and ischemia-reperfusion-injured grafts. Second, to assess the LiMAx test, as a CYP 1A2 point- of care diagnostic, the in vivo and in vitro CYP measurements are correlated. The experimental results are related to the patient outcome, especially the prevalence of delayed graft function, as well as validated clinical chemistry parameters.
+40 patients undergoing a liver transplantation in 2022/23 at university hospital in Jena, who are giving their informed consent, will be examined. For an exploratory approach, with 10 subjects each independent variable, are needed.
+With the tissue samples we perform an H.E. staining for the morphological analysis of the donor organs. Indirect immunohistochemistry for CYP expression, precisely CYP 1A2, CYP 3A4, CYP 2C19 and a fluorescent assay measuring the CYP 1A2 activity in vitro, as well as a breath test (LiMAx) to measure the CYP activity in vivo. 
+Results: 
+The CYP enzymes are expressed pericentral in the lobules. Steatosis, age, and CIT are three interrelated factors, that we predict, will influence the CYP expression pattern. We assume that the CYP activity is altered by the reperfusion and the IRI. 
+Conclusion: 
+Potentially, the LiMAx could be used to assess recovery after transplantation, reflecting the IRI.
+</t>
+  </si>
+  <si>
+    <t>Journal of Hepatology 2023 vol. 78(S1)</t>
+  </si>
+  <si>
+    <t>EASL European Association for the Study of the Liver, https://www.easlcongress.eu,</t>
+  </si>
+  <si>
+    <t>6/24/2023</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1TWLwOLSOiOVMJbJDWcqiWeXDcStcu0Ql</t>
+  </si>
+  <si>
+    <t>Bütow L.B., Tautenhahn H.-M. T., Schröter D.S., Dahmen U.D.,</t>
+  </si>
+  <si>
+    <t>P2 - Dahmen, P9 - Tautenhahn, SimLivA</t>
+  </si>
+  <si>
+    <t>Laura.buetow@uni-jena.de</t>
+  </si>
+  <si>
+    <t>Influence of marginal organs on the drug metabolism in liver transplantation. Outline for a prospective clinical study</t>
+  </si>
+  <si>
+    <t>Bütow L.B., Schröter D.S., Tautenhahn H.-M. T., Dahmen U.D., Nickel S. N.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background:
+Due to the lack of donor organs there is an increasing use of non-optimal organs. These are organs from aged donors, with steatosis or organs subjected to prolonged cold ischemia. 
+Those factors might influence the recovery of function after transplantation and thereby affect outcome. 
+One of the key functions of the liver is the drug metabolism. Ex-vivo assessment of drug metabolism includes the visualization of the key drug metabolizing CYP enzymes and the determination of the enzyme activity. In-vivo assessment of CYP 1A2 metabolism is performed using a breath test (LiMAx) after injecting a test drug (Methacetin) and is accepted as a correlate of hepatic function.
+Hypothesis:
+We hypothesize that the three factors Steatosis, age, and CIT may influence drug metabolism in liver grafts after transplantation. 
+Objective and Methods:
+We want to investigate the impact of age, steatosis and cold ischemia time on expression and activity of CYP enzymes in tissue samples obtained from liver grafts at the end of cold ischemia and 1 hour after reperfusion. First, Severity of steatosis will be determined based on HE-staining of the liver samples. Second, CYP expression will be visualized using IHC. Third, CYP activity will be assessed using a fluorescent assay. As a fourth and thus clinical part, the CYP 1A2 activity in vivo is investigated with the LiMAx.
+Wetlab results will be compared to the postoperative course of the patient with special attention to the recovery of hepatic function as determined using the LiMAx assay on POD 1 and POD 7. 
+Based on statistical the considerations of Peduzzi et al., 10 patients per individual variable should be included for an explorative approach to assess factors influencing liver function.
+Results:
+Over the time period from January 2022 until March of 2023, 40 patients were included in the study. Donor age ranged from 23 to 88 years with a mean of 59.5 years. The mean CIT was 6.13 hours. The Limax test, as illustrated by a single case so far, demonstrated the posttransplant reduced hepatic function as well as the almost complete recovery within the first postoperative week. The patient was an 59 old male with ethyl toxic liver cirrhosis who gets an 65 year old organ with a CIT time of 8 h 51. 
+</t>
+  </si>
+  <si>
+    <t>33., Wilseder Workshop von Biotest- Individulaisierte Therapie von Lebererkrnakungen, https://www.biotest-wilsede.de,</t>
+  </si>
+  <si>
+    <t>6/28/2023</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=15cC4u3YZviFf4gxS6wxKJUDcqgC3ZRZR</t>
+  </si>
+  <si>
+    <t>Bütow L.B., Schröter D.S., Tautenhahn H.-M. T., Dahmen U.D.,</t>
   </si>
 </sst>
 </file>
@@ -4118,7 +4194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="408" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>44427.977659027798</v>
       </c>
@@ -4161,7 +4237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="408" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>44427.979484606498</v>
       </c>
@@ -5203,7 +5279,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
         <v>44664.614628935196</v>
       </c>
@@ -5723,7 +5799,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A48" s="16">
         <v>44714.631931828699</v>
       </c>
@@ -5767,7 +5843,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="408" x14ac:dyDescent="0.2">
       <c r="A49" s="16">
         <v>44721.479891666699</v>
       </c>
@@ -5814,7 +5890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="331.5" x14ac:dyDescent="0.2">
       <c r="A50" s="16">
         <v>44724.908495023199</v>
       </c>
@@ -6432,7 +6508,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A65" s="16">
         <v>44769.6992456019</v>
       </c>
@@ -7068,7 +7144,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <v>44858.360405555599</v>
       </c>
@@ -7217,7 +7293,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="382.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="369.75" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>44875.441085763901</v>
       </c>
@@ -7281,7 +7357,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="16">
         <v>44875.453703819403</v>
       </c>
@@ -7489,7 +7565,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>44929.354307870402</v>
       </c>
@@ -7530,7 +7606,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A92" s="16">
         <v>44943.356896874997</v>
       </c>
@@ -8183,7 +8259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:24" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:24" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A109" s="16">
         <v>45012.448258796299</v>
       </c>
@@ -10956,7 +11032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
@@ -21600,9 +21676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ163"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24610,57 +24686,113 @@
       <c r="Z72" s="46"/>
       <c r="AA72" s="46"/>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="8"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="8"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="9"/>
-      <c r="S73" s="9"/>
-      <c r="T73" s="9"/>
-      <c r="U73" s="9"/>
-      <c r="V73" s="9"/>
-      <c r="W73" s="9"/>
-      <c r="X73" s="9"/>
-    </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
-      <c r="M74" s="8"/>
-      <c r="N74" s="8"/>
-      <c r="O74" s="8"/>
-      <c r="P74" s="8"/>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="9"/>
-      <c r="S74" s="9"/>
-      <c r="T74" s="9"/>
-      <c r="U74" s="9"/>
-      <c r="V74" s="9"/>
-      <c r="W74" s="9"/>
-      <c r="X74" s="9"/>
+    <row r="73" spans="1:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="53">
+        <v>45084.756689814814</v>
+      </c>
+      <c r="B73" s="46" t="s">
+        <v>800</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="D73" s="46" t="s">
+        <v>801</v>
+      </c>
+      <c r="E73" s="46" t="s">
+        <v>802</v>
+      </c>
+      <c r="F73" s="46" t="s">
+        <v>803</v>
+      </c>
+      <c r="G73" s="46" t="s">
+        <v>804</v>
+      </c>
+      <c r="H73" s="46" t="s">
+        <v>805</v>
+      </c>
+      <c r="I73" s="48" t="s">
+        <v>806</v>
+      </c>
+      <c r="J73" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K73" s="49" t="s">
+        <v>807</v>
+      </c>
+      <c r="L73" s="47" t="s">
+        <v>808</v>
+      </c>
+      <c r="M73" s="46"/>
+      <c r="N73" s="46"/>
+      <c r="O73" s="46"/>
+      <c r="P73" s="46"/>
+      <c r="Q73" s="47" t="s">
+        <v>809</v>
+      </c>
+      <c r="R73" s="46"/>
+      <c r="S73" s="46"/>
+      <c r="T73" s="46"/>
+      <c r="U73" s="46"/>
+      <c r="V73" s="46"/>
+      <c r="W73" s="46"/>
+      <c r="X73" s="46"/>
+      <c r="Y73" s="46"/>
+      <c r="Z73" s="46"/>
+      <c r="AA73" s="46"/>
+    </row>
+    <row r="74" spans="1:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="53">
+        <v>45084.761666666665</v>
+      </c>
+      <c r="B74" s="46" t="s">
+        <v>810</v>
+      </c>
+      <c r="C74" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" s="46" t="s">
+        <v>811</v>
+      </c>
+      <c r="E74" s="46" t="s">
+        <v>812</v>
+      </c>
+      <c r="F74" s="47" t="s">
+        <v>813</v>
+      </c>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46" t="s">
+        <v>814</v>
+      </c>
+      <c r="I74" s="48" t="s">
+        <v>815</v>
+      </c>
+      <c r="J74" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K74" s="49" t="s">
+        <v>816</v>
+      </c>
+      <c r="L74" s="47" t="s">
+        <v>817</v>
+      </c>
+      <c r="M74" s="46"/>
+      <c r="N74" s="46"/>
+      <c r="O74" s="46"/>
+      <c r="P74" s="46"/>
+      <c r="Q74" s="47" t="s">
+        <v>809</v>
+      </c>
+      <c r="R74" s="46"/>
+      <c r="S74" s="46"/>
+      <c r="T74" s="46"/>
+      <c r="U74" s="46"/>
+      <c r="V74" s="46"/>
+      <c r="W74" s="46"/>
+      <c r="X74" s="46"/>
+      <c r="Y74" s="46"/>
+      <c r="Z74" s="46"/>
+      <c r="AA74" s="46"/>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
@@ -27018,9 +27150,11 @@
     <hyperlink ref="K68" r:id="rId37" xr:uid="{1EE4AB64-2688-44A9-8FE2-0DC1279B7409}"/>
     <hyperlink ref="K72" r:id="rId38" xr:uid="{E99CE995-67FE-4E83-A47A-ECB6DA84F0D8}"/>
     <hyperlink ref="R72" r:id="rId39" xr:uid="{BE77A5A7-22A1-4438-AA52-A616D0D2F735}"/>
+    <hyperlink ref="K73" r:id="rId40" xr:uid="{28063AC0-2663-4695-9D66-4C7B825735EE}"/>
+    <hyperlink ref="K74" r:id="rId41" xr:uid="{EA44B343-679D-469F-A6FF-8811CC28240C}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId40"/>
-  <legacyDrawing r:id="rId41"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId42"/>
+  <legacyDrawing r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>